<commit_message>
tidying up the final screening
</commit_message>
<xml_diff>
--- a/lit-search/2021-06-07-final-screening.xlsx
+++ b/lit-search/2021-06-07-final-screening.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe.sharepoint.com/sites/GK-research/Shared Documents/2021 CJ meta-analysis/lit-search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1521" documentId="13_ncr:1_{B6E9A696-9688-4C1D-9F8B-DD25221004E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD8057DF-592B-4CAB-A69D-46FBD8F65290}"/>
+  <xr:revisionPtr revIDLastSave="1524" documentId="13_ncr:1_{B6E9A696-9688-4C1D-9F8B-DD25221004E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BE0408A-75F3-47EC-BE7D-ECBE7ACCD9D7}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coding" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="9086" r:id="rId6"/>
-    <pivotCache cacheId="9087" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3739" uniqueCount="1432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3738" uniqueCount="1432">
   <si>
     <t>bibtexkey</t>
   </si>
@@ -4993,7 +4993,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -13140,7 +13140,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8E93CBB0-DC61-4995-BE94-9568EC1373AA}" name="PivotTable1" cacheId="9086" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8E93CBB0-DC61-4995-BE94-9568EC1373AA}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField dataField="1" showAll="0"/>
@@ -13267,7 +13267,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{744EC8D8-32F1-49F3-9F75-8076F492AF88}" name="PivotTable1" cacheId="9087" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{744EC8D8-32F1-49F3-9F75-8076F492AF88}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B68" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="17">
     <pivotField dataField="1" showAll="0"/>
@@ -13996,30 +13996,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="44.5703125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.1328125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="44.59765625" style="4" customWidth="1"/>
     <col min="3" max="3" width="9" style="4"/>
-    <col min="4" max="4" width="46.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.42578125" customWidth="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1"/>
-    <col min="12" max="12" width="26.140625" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" customWidth="1"/>
-    <col min="14" max="17" width="16.85546875" customWidth="1"/>
-    <col min="18" max="18" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46.3984375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.3984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.3984375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="9.59765625" customWidth="1"/>
+    <col min="8" max="8" width="11.3984375" customWidth="1"/>
+    <col min="9" max="9" width="36.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.3984375" customWidth="1"/>
+    <col min="11" max="11" width="26.265625" customWidth="1"/>
+    <col min="12" max="12" width="26.1328125" customWidth="1"/>
+    <col min="13" max="13" width="16.3984375" customWidth="1"/>
+    <col min="14" max="17" width="16.86328125" customWidth="1"/>
+    <col min="18" max="18" width="12.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -14081,7 +14081,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="26.65">
+    <row r="2" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -14131,7 +14131,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="26.65">
+    <row r="3" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>34</v>
       </c>
@@ -14184,7 +14184,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="26.65">
+    <row r="4" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>46</v>
       </c>
@@ -14237,7 +14237,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="39.75">
+    <row r="5" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>52</v>
       </c>
@@ -14296,7 +14296,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="26.65">
+    <row r="6" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>65</v>
       </c>
@@ -14352,7 +14352,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="26.65">
+    <row r="7" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>75</v>
       </c>
@@ -14402,7 +14402,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="26.65">
+    <row r="8" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>84</v>
       </c>
@@ -14461,7 +14461,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="39.75">
+    <row r="9" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>95</v>
       </c>
@@ -14520,7 +14520,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="26.65">
+    <row r="10" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>105</v>
       </c>
@@ -14579,7 +14579,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="26.65">
+    <row r="11" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>116</v>
       </c>
@@ -14638,7 +14638,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="39.75">
+    <row r="12" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>126</v>
       </c>
@@ -14694,7 +14694,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="26.65">
+    <row r="13" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>136</v>
       </c>
@@ -14744,7 +14744,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="26.65">
+    <row r="14" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>145</v>
       </c>
@@ -14797,7 +14797,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="26.65">
+    <row r="15" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>154</v>
       </c>
@@ -14856,7 +14856,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="39.75">
+    <row r="16" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>163</v>
       </c>
@@ -14909,7 +14909,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="39.75">
+    <row r="17" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>172</v>
       </c>
@@ -14968,7 +14968,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="26.65">
+    <row r="18" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
         <v>181</v>
       </c>
@@ -15027,7 +15027,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="26.65">
+    <row r="19" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
         <v>192</v>
       </c>
@@ -15083,7 +15083,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="26.65">
+    <row r="20" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
         <v>202</v>
       </c>
@@ -15142,7 +15142,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>211</v>
       </c>
@@ -15179,9 +15179,6 @@
       <c r="L21" t="s">
         <v>218</v>
       </c>
-      <c r="M21" t="s">
-        <v>26</v>
-      </c>
       <c r="N21" s="17">
         <v>44477</v>
       </c>
@@ -15195,7 +15192,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="26.65">
+    <row r="22" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
         <v>220</v>
       </c>
@@ -15254,7 +15251,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
         <v>230</v>
       </c>
@@ -15304,7 +15301,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="26.65">
+    <row r="24" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
         <v>239</v>
       </c>
@@ -15354,7 +15351,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="26.65">
+    <row r="25" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
         <v>247</v>
       </c>
@@ -15410,7 +15407,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="26.65">
+    <row r="26" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
         <v>256</v>
       </c>
@@ -15469,7 +15466,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
         <v>267</v>
       </c>
@@ -15522,7 +15519,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="26.65">
+    <row r="28" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
         <v>277</v>
       </c>
@@ -15575,7 +15572,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
         <v>286</v>
       </c>
@@ -15631,7 +15628,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.45">
       <c r="B30" s="4" t="s">
         <v>287</v>
       </c>
@@ -15667,7 +15664,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="26.65">
+    <row r="31" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="s">
         <v>296</v>
       </c>
@@ -15720,7 +15717,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="26.65">
+    <row r="32" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
         <v>306</v>
       </c>
@@ -15776,7 +15773,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="26.65">
+    <row r="33" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="s">
         <v>316</v>
       </c>
@@ -15829,7 +15826,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="26.65">
+    <row r="34" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A34" s="4" t="s">
         <v>325</v>
       </c>
@@ -15882,7 +15879,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="39.75">
+    <row r="35" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A35" s="4" t="s">
         <v>331</v>
       </c>
@@ -15938,7 +15935,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="26.65">
+    <row r="36" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="s">
         <v>341</v>
       </c>
@@ -15994,7 +15991,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="26.65">
+    <row r="37" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
         <v>351</v>
       </c>
@@ -16050,7 +16047,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="39.75">
+    <row r="38" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A38" s="4" t="s">
         <v>360</v>
       </c>
@@ -16103,7 +16100,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="26.65">
+    <row r="39" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A39" s="4" t="s">
         <v>366</v>
       </c>
@@ -16156,7 +16153,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="52.9">
+    <row r="40" spans="1:20" ht="52.9" x14ac:dyDescent="0.45">
       <c r="A40" s="4" t="s">
         <v>372</v>
       </c>
@@ -16212,7 +16209,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="26.65">
+    <row r="41" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="s">
         <v>379</v>
       </c>
@@ -16262,7 +16259,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="26.65">
+    <row r="42" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="s">
         <v>387</v>
       </c>
@@ -16318,7 +16315,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="26.65">
+    <row r="43" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="s">
         <v>397</v>
       </c>
@@ -16374,7 +16371,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="39.75">
+    <row r="44" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="s">
         <v>404</v>
       </c>
@@ -16427,7 +16424,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="26.65">
+    <row r="45" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
         <v>410</v>
       </c>
@@ -16483,7 +16480,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="39.75">
+    <row r="46" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A46" s="4" t="s">
         <v>417</v>
       </c>
@@ -16536,7 +16533,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="39.75">
+    <row r="47" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A47" s="4" t="s">
         <v>423</v>
       </c>
@@ -16595,7 +16592,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="26.65">
+    <row r="48" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="s">
         <v>431</v>
       </c>
@@ -16651,7 +16648,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="26.65">
+    <row r="49" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A49" s="4" t="s">
         <v>438</v>
       </c>
@@ -16707,7 +16704,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="26.65">
+    <row r="50" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A50" s="4" t="s">
         <v>445</v>
       </c>
@@ -16763,7 +16760,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="26.65">
+    <row r="51" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A51" s="4" t="s">
         <v>455</v>
       </c>
@@ -16816,7 +16813,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.45">
       <c r="B52" s="4" t="s">
         <v>464</v>
       </c>
@@ -16848,7 +16845,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="26.65">
+    <row r="53" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A53" s="4" t="s">
         <v>469</v>
       </c>
@@ -16901,7 +16898,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="39.75">
+    <row r="54" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A54" s="4" t="s">
         <v>479</v>
       </c>
@@ -16960,7 +16957,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="55" spans="1:20" s="12" customFormat="1" ht="26.65">
+    <row r="55" spans="1:20" s="12" customFormat="1" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A55" s="4" t="s">
         <v>490</v>
       </c>
@@ -17016,7 +17013,7 @@
       <c r="S55"/>
       <c r="T55"/>
     </row>
-    <row r="56" spans="1:20" s="12" customFormat="1" ht="26.65">
+    <row r="56" spans="1:20" s="12" customFormat="1" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A56" s="4" t="s">
         <v>499</v>
       </c>
@@ -17076,7 +17073,7 @@
       </c>
       <c r="T56"/>
     </row>
-    <row r="57" spans="1:20">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A57" s="4" t="s">
         <v>510</v>
       </c>
@@ -17132,7 +17129,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="58" spans="1:20">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.45">
       <c r="B58" s="4" t="s">
         <v>520</v>
       </c>
@@ -17171,7 +17168,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A59" s="4" t="s">
         <v>522</v>
       </c>
@@ -17227,7 +17224,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="26.65">
+    <row r="60" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A60" s="10" t="s">
         <v>531</v>
       </c>
@@ -17285,7 +17282,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="61" spans="1:20">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A61" s="10" t="s">
         <v>538</v>
       </c>
@@ -17343,7 +17340,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="26.65">
+    <row r="62" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A62" s="4" t="s">
         <v>544</v>
       </c>
@@ -17396,7 +17393,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="26.65">
+    <row r="63" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A63" s="4" t="s">
         <v>554</v>
       </c>
@@ -17446,7 +17443,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="26.65">
+    <row r="64" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A64" s="4" t="s">
         <v>563</v>
       </c>
@@ -17493,7 +17490,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="26.65">
+    <row r="65" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A65" s="4" t="s">
         <v>567</v>
       </c>
@@ -17552,7 +17549,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="39.75">
+    <row r="66" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A66" s="4" t="s">
         <v>577</v>
       </c>
@@ -17602,7 +17599,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="26.65">
+    <row r="67" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A67" s="4" t="s">
         <v>586</v>
       </c>
@@ -17649,7 +17646,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="39.75">
+    <row r="68" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A68" s="4" t="s">
         <v>593</v>
       </c>
@@ -17699,7 +17696,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="39.75">
+    <row r="69" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A69" s="4" t="s">
         <v>599</v>
       </c>
@@ -17746,7 +17743,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="39.75">
+    <row r="70" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A70" s="4" t="s">
         <v>602</v>
       </c>
@@ -17796,7 +17793,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="39.75">
+    <row r="71" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A71" s="4" t="s">
         <v>608</v>
       </c>
@@ -17852,7 +17849,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="26.65">
+    <row r="72" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A72" s="4" t="s">
         <v>619</v>
       </c>
@@ -17908,7 +17905,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="26.65">
+    <row r="73" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A73" s="4" t="s">
         <v>624</v>
       </c>
@@ -17958,7 +17955,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="26.65">
+    <row r="74" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A74" s="4" t="s">
         <v>631</v>
       </c>
@@ -18011,7 +18008,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="26.65">
+    <row r="75" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A75" s="4" t="s">
         <v>639</v>
       </c>
@@ -18064,7 +18061,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="26.65">
+    <row r="76" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A76" s="4" t="s">
         <v>644</v>
       </c>
@@ -18120,7 +18117,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="26.65">
+    <row r="77" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A77" s="4" t="s">
         <v>650</v>
       </c>
@@ -18173,7 +18170,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="26.65">
+    <row r="78" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A78" s="4" t="s">
         <v>658</v>
       </c>
@@ -18229,7 +18226,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="26.65">
+    <row r="79" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A79" s="4" t="s">
         <v>669</v>
       </c>
@@ -18288,7 +18285,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="39.75">
+    <row r="80" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A80" s="4" t="s">
         <v>679</v>
       </c>
@@ -18347,7 +18344,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="26.65">
+    <row r="81" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A81" s="4" t="s">
         <v>686</v>
       </c>
@@ -18397,7 +18394,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="26.65">
+    <row r="82" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A82" s="4" t="s">
         <v>694</v>
       </c>
@@ -18453,7 +18450,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="39.75">
+    <row r="83" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A83" s="4" t="s">
         <v>703</v>
       </c>
@@ -18506,7 +18503,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="39.75">
+    <row r="84" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A84" s="4" t="s">
         <v>711</v>
       </c>
@@ -18556,7 +18553,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="26.65">
+    <row r="85" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A85" s="4" t="s">
         <v>720</v>
       </c>
@@ -18615,7 +18612,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="26.65">
+    <row r="86" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A86" s="4" t="s">
         <v>728</v>
       </c>
@@ -18668,7 +18665,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="39.75">
+    <row r="87" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A87" s="4" t="s">
         <v>736</v>
       </c>
@@ -18718,7 +18715,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="26.65">
+    <row r="88" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A88" s="4" t="s">
         <v>744</v>
       </c>
@@ -18768,7 +18765,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="26.65">
+    <row r="89" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A89" s="4" t="s">
         <v>750</v>
       </c>
@@ -18804,7 +18801,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="26.65">
+    <row r="90" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A90" s="4" t="s">
         <v>756</v>
       </c>
@@ -18857,7 +18854,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="26.65">
+    <row r="91" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A91" s="4" t="s">
         <v>761</v>
       </c>
@@ -18913,7 +18910,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="26.65">
+    <row r="92" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A92" s="4" t="s">
         <v>770</v>
       </c>
@@ -18963,7 +18960,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="39.75">
+    <row r="93" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A93" s="4" t="s">
         <v>779</v>
       </c>
@@ -19013,7 +19010,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="94" spans="1:19">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A94" s="4" t="s">
         <v>784</v>
       </c>
@@ -19066,7 +19063,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="26.65">
+    <row r="95" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A95" s="4" t="s">
         <v>793</v>
       </c>
@@ -19116,7 +19113,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="26.65">
+    <row r="96" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A96" s="4" t="s">
         <v>798</v>
       </c>
@@ -19169,7 +19166,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="97" spans="1:20">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A97" s="4" t="s">
         <v>804</v>
       </c>
@@ -19222,7 +19219,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="26.65">
+    <row r="98" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A98" s="4" t="s">
         <v>810</v>
       </c>
@@ -19275,7 +19272,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="99" spans="1:20">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A99" s="4" t="s">
         <v>816</v>
       </c>
@@ -19328,7 +19325,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="100" spans="1:20">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A100" s="4" t="s">
         <v>822</v>
       </c>
@@ -19378,7 +19375,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="26.65">
+    <row r="101" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A101" s="4" t="s">
         <v>827</v>
       </c>
@@ -19431,7 +19428,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="26.65">
+    <row r="102" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A102" s="4" t="s">
         <v>833</v>
       </c>
@@ -19481,7 +19478,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="26.65">
+    <row r="103" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A103" s="4" t="s">
         <v>838</v>
       </c>
@@ -19534,7 +19531,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="26.65">
+    <row r="104" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A104" s="4" t="s">
         <v>844</v>
       </c>
@@ -19587,7 +19584,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="26.65">
+    <row r="105" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A105" s="4" t="s">
         <v>850</v>
       </c>
@@ -19631,7 +19628,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="26.65">
+    <row r="106" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A106" s="4" t="s">
         <v>856</v>
       </c>
@@ -19678,7 +19675,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="39.75">
+    <row r="107" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A107" s="4" t="s">
         <v>862</v>
       </c>
@@ -19722,7 +19719,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="26.65">
+    <row r="108" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A108" s="4" t="s">
         <v>867</v>
       </c>
@@ -19769,7 +19766,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="26.65">
+    <row r="109" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A109" s="4" t="s">
         <v>873</v>
       </c>
@@ -19810,7 +19807,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="39.75">
+    <row r="110" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A110" s="4" t="s">
         <v>877</v>
       </c>
@@ -19840,7 +19837,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="111" spans="1:20">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A111" s="4" t="s">
         <v>883</v>
       </c>
@@ -19873,7 +19870,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="26.65">
+    <row r="112" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A112" s="4" t="s">
         <v>887</v>
       </c>
@@ -19903,7 +19900,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="26.65">
+    <row r="113" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A113" s="4" t="s">
         <v>891</v>
       </c>
@@ -19933,7 +19930,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="26.65">
+    <row r="114" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A114" s="4" t="s">
         <v>896</v>
       </c>
@@ -19966,7 +19963,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="26.65">
+    <row r="115" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A115" s="4" t="s">
         <v>902</v>
       </c>
@@ -19999,7 +19996,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="116" spans="1:19">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A116" s="4" t="s">
         <v>908</v>
       </c>
@@ -20026,7 +20023,7 @@
       </c>
       <c r="J116" s="4"/>
     </row>
-    <row r="117" spans="1:19" ht="26.65">
+    <row r="117" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A117" s="4" t="s">
         <v>911</v>
       </c>
@@ -20059,7 +20056,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="26.65">
+    <row r="118" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A118" s="4" t="s">
         <v>916</v>
       </c>
@@ -20089,7 +20086,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="39.75">
+    <row r="119" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A119" s="4" t="s">
         <v>921</v>
       </c>
@@ -20122,7 +20119,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="26.65">
+    <row r="120" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A120" s="4" t="s">
         <v>927</v>
       </c>
@@ -20155,7 +20152,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="39.75">
+    <row r="121" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A121" s="4" t="s">
         <v>932</v>
       </c>
@@ -20188,7 +20185,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="26.65">
+    <row r="122" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A122" s="4" t="s">
         <v>936</v>
       </c>
@@ -20218,7 +20215,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="26.65">
+    <row r="123" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A123" s="4" t="s">
         <v>941</v>
       </c>
@@ -20248,7 +20245,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="124" spans="1:19" ht="26.65">
+    <row r="124" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A124" s="4" t="s">
         <v>946</v>
       </c>
@@ -20281,7 +20278,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="125" spans="1:19" ht="39.75">
+    <row r="125" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A125" s="4" t="s">
         <v>952</v>
       </c>
@@ -20311,7 +20308,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="126" spans="1:19" ht="26.65">
+    <row r="126" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A126" s="4" t="s">
         <v>956</v>
       </c>
@@ -20341,7 +20338,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="39.75">
+    <row r="127" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A127" s="4" t="s">
         <v>960</v>
       </c>
@@ -20371,7 +20368,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="39.75">
+    <row r="128" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A128" s="4" t="s">
         <v>964</v>
       </c>
@@ -20398,7 +20395,7 @@
       </c>
       <c r="J128" s="4"/>
     </row>
-    <row r="129" spans="1:19" ht="39.75">
+    <row r="129" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A129" s="4" t="s">
         <v>968</v>
       </c>
@@ -20431,7 +20428,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="26.65">
+    <row r="130" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A130" s="4" t="s">
         <v>973</v>
       </c>
@@ -20464,7 +20461,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="26.65">
+    <row r="131" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A131" s="4" t="s">
         <v>978</v>
       </c>
@@ -20497,7 +20494,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="26.65">
+    <row r="132" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A132" s="4" t="s">
         <v>983</v>
       </c>
@@ -20527,7 +20524,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="26.65">
+    <row r="133" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A133" s="4" t="s">
         <v>988</v>
       </c>
@@ -20560,7 +20557,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="134" spans="1:19" ht="26.65">
+    <row r="134" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A134" s="4" t="s">
         <v>994</v>
       </c>
@@ -20590,7 +20587,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="39.75">
+    <row r="135" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A135" s="4" t="s">
         <v>1000</v>
       </c>
@@ -20620,7 +20617,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="26.65">
+    <row r="136" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A136" s="4" t="s">
         <v>1004</v>
       </c>
@@ -20650,7 +20647,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="137" spans="1:19" ht="26.65">
+    <row r="137" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A137" s="4" t="s">
         <v>1007</v>
       </c>
@@ -20683,7 +20680,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="26.65">
+    <row r="138" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A138" s="4" t="s">
         <v>1013</v>
       </c>
@@ -20713,7 +20710,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="139" spans="1:19" ht="26.65">
+    <row r="139" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A139" s="4" t="s">
         <v>1017</v>
       </c>
@@ -20743,7 +20740,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="26.65">
+    <row r="140" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A140" s="4" t="s">
         <v>1021</v>
       </c>
@@ -20776,7 +20773,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="39.75">
+    <row r="141" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A141" s="4" t="s">
         <v>1027</v>
       </c>
@@ -20803,7 +20800,7 @@
       </c>
       <c r="J141" s="4"/>
     </row>
-    <row r="142" spans="1:19" ht="26.65">
+    <row r="142" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A142" s="4" t="s">
         <v>1029</v>
       </c>
@@ -20833,7 +20830,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="26.65">
+    <row r="143" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A143" s="4" t="s">
         <v>1034</v>
       </c>
@@ -20863,7 +20860,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="26.65">
+    <row r="144" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A144" s="4" t="s">
         <v>1039</v>
       </c>
@@ -20896,7 +20893,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="39.75">
+    <row r="145" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A145" s="4" t="s">
         <v>1044</v>
       </c>
@@ -20929,7 +20926,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="146" spans="1:20">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A146" s="4" t="s">
         <v>1048</v>
       </c>
@@ -20956,7 +20953,7 @@
       </c>
       <c r="J146" s="4"/>
     </row>
-    <row r="147" spans="1:20" ht="26.65">
+    <row r="147" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A147" s="4" t="s">
         <v>1053</v>
       </c>
@@ -20986,7 +20983,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="39.75">
+    <row r="148" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A148" s="4" t="s">
         <v>1058</v>
       </c>
@@ -21015,7 +21012,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="26.65">
+    <row r="149" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A149" s="4" t="s">
         <v>1063</v>
       </c>
@@ -21048,7 +21045,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="26.65">
+    <row r="150" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A150" s="4" t="s">
         <v>1069</v>
       </c>
@@ -21081,7 +21078,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="26.65">
+    <row r="151" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A151" s="4" t="s">
         <v>1075</v>
       </c>
@@ -21128,7 +21125,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="26.65">
+    <row r="152" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A152" s="4" t="s">
         <v>1081</v>
       </c>
@@ -21178,7 +21175,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="26.65">
+    <row r="153" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A153" s="4" t="s">
         <v>1087</v>
       </c>
@@ -21225,7 +21222,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="154" spans="1:20">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A154" s="4" t="s">
         <v>1091</v>
       </c>
@@ -21272,7 +21269,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="39.75">
+    <row r="155" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A155" s="4" t="s">
         <v>1096</v>
       </c>
@@ -21316,7 +21313,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="26.65">
+    <row r="156" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A156" s="4" t="s">
         <v>1100</v>
       </c>
@@ -21349,7 +21346,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="26.65">
+    <row r="157" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A157" s="4" t="s">
         <v>1106</v>
       </c>
@@ -21379,7 +21376,7 @@
       </c>
       <c r="J157" s="4"/>
     </row>
-    <row r="158" spans="1:20" ht="26.65">
+    <row r="158" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A158" s="4" t="s">
         <v>1111</v>
       </c>
@@ -21409,7 +21406,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="39.75">
+    <row r="159" spans="1:20" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A159" s="4" t="s">
         <v>1116</v>
       </c>
@@ -21442,7 +21439,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="26.65">
+    <row r="160" spans="1:20" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A160" s="4" t="s">
         <v>1122</v>
       </c>
@@ -21475,7 +21472,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="161" spans="1:19">
+    <row r="161" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A161" s="4" t="s">
         <v>1128</v>
       </c>
@@ -21508,7 +21505,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="162" spans="1:19" ht="26.65">
+    <row r="162" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A162" s="4" t="s">
         <v>1133</v>
       </c>
@@ -21541,7 +21538,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="163" spans="1:19">
+    <row r="163" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A163" s="4" t="s">
         <v>1139</v>
       </c>
@@ -21574,7 +21571,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="164" spans="1:19" ht="26.65">
+    <row r="164" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A164" s="4" t="s">
         <v>1145</v>
       </c>
@@ -21604,7 +21601,7 @@
       </c>
       <c r="J164" s="4"/>
     </row>
-    <row r="165" spans="1:19">
+    <row r="165" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A165" s="4" t="s">
         <v>1150</v>
       </c>
@@ -21637,7 +21634,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="166" spans="1:19" ht="26.65">
+    <row r="166" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A166" s="4" t="s">
         <v>1155</v>
       </c>
@@ -21670,7 +21667,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="167" spans="1:19" ht="26.65">
+    <row r="167" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A167" s="4" t="s">
         <v>1161</v>
       </c>
@@ -21703,7 +21700,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="26.65">
+    <row r="168" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A168" s="4" t="s">
         <v>1166</v>
       </c>
@@ -21733,7 +21730,7 @@
       </c>
       <c r="J168" s="4"/>
     </row>
-    <row r="169" spans="1:19">
+    <row r="169" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A169" s="4" t="s">
         <v>1171</v>
       </c>
@@ -21766,7 +21763,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="170" spans="1:19" ht="26.65">
+    <row r="170" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A170" s="4" t="s">
         <v>1176</v>
       </c>
@@ -21799,7 +21796,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="171" spans="1:19">
+    <row r="171" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A171" s="4" t="s">
         <v>1182</v>
       </c>
@@ -21832,7 +21829,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="172" spans="1:19" ht="26.65">
+    <row r="172" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A172" s="4" t="s">
         <v>1187</v>
       </c>
@@ -21868,7 +21865,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="173" spans="1:19" ht="39.75">
+    <row r="173" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A173" s="4" t="s">
         <v>1192</v>
       </c>
@@ -21898,7 +21895,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="174" spans="1:19" ht="39.75">
+    <row r="174" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A174" s="4" t="s">
         <v>1197</v>
       </c>
@@ -21931,7 +21928,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="175" spans="1:19" ht="26.65">
+    <row r="175" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A175" s="4" t="s">
         <v>1203</v>
       </c>
@@ -21961,7 +21958,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="176" spans="1:19" ht="26.65">
+    <row r="176" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A176" s="4" t="s">
         <v>1208</v>
       </c>
@@ -21994,7 +21991,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="177" spans="1:19" ht="26.65">
+    <row r="177" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A177" s="4" t="s">
         <v>1214</v>
       </c>
@@ -22027,7 +22024,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="178" spans="1:19" ht="26.65">
+    <row r="178" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A178" s="4" t="s">
         <v>1219</v>
       </c>
@@ -22057,7 +22054,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="179" spans="1:19">
+    <row r="179" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A179" s="4" t="s">
         <v>1224</v>
       </c>
@@ -22093,7 +22090,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="180" spans="1:19" ht="39.75">
+    <row r="180" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A180" s="4" t="s">
         <v>1228</v>
       </c>
@@ -22126,7 +22123,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="181" spans="1:19" ht="26.65">
+    <row r="181" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A181" s="4" t="s">
         <v>1233</v>
       </c>
@@ -22156,7 +22153,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="182" spans="1:19">
+    <row r="182" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A182" s="4" t="s">
         <v>1237</v>
       </c>
@@ -22189,7 +22186,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="183" spans="1:19" ht="26.65">
+    <row r="183" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A183" s="4" t="s">
         <v>1242</v>
       </c>
@@ -22222,7 +22219,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="184" spans="1:19" ht="26.65">
+    <row r="184" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A184" s="4" t="s">
         <v>1248</v>
       </c>
@@ -22255,7 +22252,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="185" spans="1:19" ht="26.65">
+    <row r="185" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A185" s="4" t="s">
         <v>1254</v>
       </c>
@@ -22288,7 +22285,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="186" spans="1:19">
+    <row r="186" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A186" s="4" t="s">
         <v>1260</v>
       </c>
@@ -22318,7 +22315,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="187" spans="1:19" ht="39.75">
+    <row r="187" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A187" s="4" t="s">
         <v>1265</v>
       </c>
@@ -22351,7 +22348,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="188" spans="1:19" ht="26.65">
+    <row r="188" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A188" s="4" t="s">
         <v>1271</v>
       </c>
@@ -22381,7 +22378,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="189" spans="1:19" ht="26.65">
+    <row r="189" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A189" s="4" t="s">
         <v>1276</v>
       </c>
@@ -22411,7 +22408,7 @@
       </c>
       <c r="J189" s="4"/>
     </row>
-    <row r="190" spans="1:19" ht="26.65">
+    <row r="190" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A190" s="4" t="s">
         <v>1281</v>
       </c>
@@ -22444,7 +22441,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="191" spans="1:19" ht="39.75">
+    <row r="191" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A191" s="4" t="s">
         <v>1287</v>
       </c>
@@ -22477,7 +22474,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="192" spans="1:19" ht="26.65">
+    <row r="192" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A192" s="4" t="s">
         <v>1293</v>
       </c>
@@ -22510,7 +22507,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="193" spans="1:19" ht="26.65">
+    <row r="193" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A193" s="4" t="s">
         <v>1298</v>
       </c>
@@ -22540,7 +22537,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="194" spans="1:19" ht="26.65">
+    <row r="194" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A194" s="4" t="s">
         <v>1303</v>
       </c>
@@ -22573,7 +22570,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="195" spans="1:19" ht="26.65">
+    <row r="195" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A195" s="4" t="s">
         <v>1308</v>
       </c>
@@ -22612,7 +22609,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="196" spans="1:19" ht="26.65">
+    <row r="196" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A196" s="4" t="s">
         <v>1313</v>
       </c>
@@ -22642,7 +22639,7 @@
       </c>
       <c r="J196" s="4"/>
     </row>
-    <row r="197" spans="1:19" ht="26.65">
+    <row r="197" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A197" s="4" t="s">
         <v>1318</v>
       </c>
@@ -22675,7 +22672,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="198" spans="1:19" ht="26.65">
+    <row r="198" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A198" s="4" t="s">
         <v>1322</v>
       </c>
@@ -22705,7 +22702,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="199" spans="1:19" ht="26.65">
+    <row r="199" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A199" s="4" t="s">
         <v>1326</v>
       </c>
@@ -22735,7 +22732,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="200" spans="1:19" ht="26.65">
+    <row r="200" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A200" s="4" t="s">
         <v>1332</v>
       </c>
@@ -22768,7 +22765,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="201" spans="1:19" ht="26.65">
+    <row r="201" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A201" s="4" t="s">
         <v>1338</v>
       </c>
@@ -22801,7 +22798,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="202" spans="1:19" ht="26.65">
+    <row r="202" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A202" s="4" t="s">
         <v>1342</v>
       </c>
@@ -22831,7 +22828,7 @@
       </c>
       <c r="J202" s="4"/>
     </row>
-    <row r="203" spans="1:19" ht="26.65">
+    <row r="203" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A203" s="4" t="s">
         <v>1347</v>
       </c>
@@ -22864,7 +22861,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="204" spans="1:19" ht="26.65">
+    <row r="204" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A204" s="4" t="s">
         <v>1352</v>
       </c>
@@ -22897,7 +22894,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="205" spans="1:19" ht="39.75">
+    <row r="205" spans="1:19" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A205" s="4" t="s">
         <v>1357</v>
       </c>
@@ -22930,7 +22927,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="206" spans="1:19" ht="26.65">
+    <row r="206" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A206" s="4" t="s">
         <v>1363</v>
       </c>
@@ -22963,7 +22960,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="207" spans="1:19" ht="26.65">
+    <row r="207" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A207" s="4" t="s">
         <v>1367</v>
       </c>
@@ -22996,7 +22993,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="208" spans="1:19" ht="26.65">
+    <row r="208" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A208" s="4" t="s">
         <v>1372</v>
       </c>
@@ -23026,7 +23023,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="209" spans="1:19" ht="26.65">
+    <row r="209" spans="1:19" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A209" s="4" t="s">
         <v>1374</v>
       </c>
@@ -23059,7 +23056,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="210" spans="1:19">
+    <row r="210" spans="1:19" x14ac:dyDescent="0.45">
       <c r="B210" s="4" t="s">
         <v>1380</v>
       </c>
@@ -23103,7 +23100,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="211" spans="1:19">
+    <row r="211" spans="1:19" x14ac:dyDescent="0.45">
       <c r="B211" s="4" t="s">
         <v>1386</v>
       </c>
@@ -23220,42 +23217,42 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.86328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.73046875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="38.73046875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="41.73046875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.1328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="25.1328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.86328125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.1328125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="27" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>1390</v>
       </c>
@@ -23263,7 +23260,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>1392</v>
       </c>
@@ -23280,7 +23277,7 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -23297,7 +23294,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>32</v>
       </c>
@@ -23314,7 +23311,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>612</v>
       </c>
@@ -23325,7 +23322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>1052</v>
       </c>
@@ -23336,7 +23333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>1394</v>
       </c>
@@ -23347,7 +23344,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>998</v>
       </c>
@@ -23358,7 +23355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
         <v>1330</v>
       </c>
@@ -23369,7 +23366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="7" t="s">
         <v>871</v>
       </c>
@@ -23380,7 +23377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="7" t="s">
         <v>981</v>
       </c>
@@ -23394,7 +23391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
         <v>881</v>
       </c>
@@ -23405,7 +23402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
         <v>967</v>
       </c>
@@ -23416,7 +23413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
         <v>1393</v>
       </c>
@@ -23446,13 +23443,13 @@
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="90.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="90.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>1392</v>
       </c>
@@ -23460,7 +23457,7 @@
         <v>1390</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
         <v>26</v>
       </c>
@@ -23468,7 +23465,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>29</v>
       </c>
@@ -23476,7 +23473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>151</v>
       </c>
@@ -23484,7 +23481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>160</v>
       </c>
@@ -23492,7 +23489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>178</v>
       </c>
@@ -23500,7 +23497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>72</v>
       </c>
@@ -23508,7 +23505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>169</v>
       </c>
@@ -23516,7 +23513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>42</v>
       </c>
@@ -23524,7 +23521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>188</v>
       </c>
@@ -23532,7 +23529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>199</v>
       </c>
@@ -23540,7 +23537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>60</v>
       </c>
@@ -23548,7 +23545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>1395</v>
       </c>
@@ -23556,7 +23553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>208</v>
       </c>
@@ -23564,7 +23561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>91</v>
       </c>
@@ -23572,7 +23569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>102</v>
       </c>
@@ -23580,7 +23577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>80</v>
       </c>
@@ -23588,7 +23585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>217</v>
       </c>
@@ -23596,7 +23593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>226</v>
       </c>
@@ -23604,7 +23601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>143</v>
       </c>
@@ -23612,7 +23609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>527</v>
       </c>
@@ -23620,7 +23617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>111</v>
       </c>
@@ -23628,7 +23625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>245</v>
       </c>
@@ -23636,7 +23633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>122</v>
       </c>
@@ -23644,7 +23641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>237</v>
       </c>
@@ -23652,7 +23649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>132</v>
       </c>
@@ -23660,7 +23657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>253</v>
       </c>
@@ -23668,7 +23665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="7" t="s">
         <v>39</v>
       </c>
@@ -23676,7 +23673,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>475</v>
       </c>
@@ -23684,7 +23681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>282</v>
       </c>
@@ -23692,7 +23689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>485</v>
       </c>
@@ -23700,7 +23697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>496</v>
       </c>
@@ -23708,7 +23705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>312</v>
       </c>
@@ -23716,7 +23713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>505</v>
       </c>
@@ -23724,7 +23721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>516</v>
       </c>
@@ -23732,7 +23729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>303</v>
       </c>
@@ -23740,7 +23737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>321</v>
       </c>
@@ -23748,7 +23745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>337</v>
       </c>
@@ -23756,7 +23753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>347</v>
       </c>
@@ -23764,7 +23761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" s="9" t="s">
         <v>273</v>
       </c>
@@ -23772,7 +23769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" s="9" t="s">
         <v>357</v>
       </c>
@@ -23780,7 +23777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" s="9" t="s">
         <v>385</v>
       </c>
@@ -23788,7 +23785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
         <v>393</v>
       </c>
@@ -23796,7 +23793,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" s="9" t="s">
         <v>451</v>
       </c>
@@ -23804,7 +23801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" s="7" t="s">
         <v>58</v>
       </c>
@@ -23812,7 +23809,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" s="9" t="s">
         <v>560</v>
       </c>
@@ -23820,7 +23817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
         <v>549</v>
       </c>
@@ -23828,7 +23825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50" s="9" t="s">
         <v>584</v>
       </c>
@@ -23836,7 +23833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" s="9" t="s">
         <v>591</v>
       </c>
@@ -23844,7 +23841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52" s="9" t="s">
         <v>614</v>
       </c>
@@ -23852,7 +23849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53" s="9" t="s">
         <v>656</v>
       </c>
@@ -23860,7 +23857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A54" s="9" t="s">
         <v>767</v>
       </c>
@@ -23868,7 +23865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
         <v>664</v>
       </c>
@@ -23876,7 +23873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56" s="9" t="s">
         <v>734</v>
       </c>
@@ -23884,7 +23881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57" s="9" t="s">
         <v>675</v>
       </c>
@@ -23892,7 +23889,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
         <v>461</v>
       </c>
@@ -23900,7 +23897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59" s="9" t="s">
         <v>691</v>
       </c>
@@ -23908,7 +23905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60" s="9" t="s">
         <v>699</v>
       </c>
@@ -23916,7 +23913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61" s="9" t="s">
         <v>709</v>
       </c>
@@ -23924,7 +23921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A62" s="9" t="s">
         <v>717</v>
       </c>
@@ -23932,7 +23929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A63" s="9" t="s">
         <v>742</v>
       </c>
@@ -23940,7 +23937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A64" s="9" t="s">
         <v>573</v>
       </c>
@@ -23948,7 +23945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65" s="7" t="s">
         <v>63</v>
       </c>
@@ -23956,7 +23953,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66" s="9" t="s">
         <v>776</v>
       </c>
@@ -23964,7 +23961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A67" s="9" t="s">
         <v>790</v>
       </c>
@@ -23972,7 +23969,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A68" s="7" t="s">
         <v>1393</v>
       </c>
@@ -23993,21 +23990,21 @@
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.59765625" customWidth="1"/>
+    <col min="7" max="7" width="9.59765625" customWidth="1"/>
+    <col min="8" max="8" width="12.265625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1"/>
-    <col min="12" max="12" width="26.140625" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="26.265625" customWidth="1"/>
+    <col min="12" max="12" width="26.1328125" customWidth="1"/>
+    <col min="13" max="13" width="13.1328125" customWidth="1"/>
+    <col min="14" max="14" width="11.265625" customWidth="1"/>
+    <col min="15" max="15" width="16.86328125" customWidth="1"/>
+    <col min="17" max="17" width="12.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -24060,7 +24057,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -24098,7 +24095,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>145</v>
       </c>
@@ -24139,7 +24136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>154</v>
       </c>
@@ -24189,7 +24186,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -24239,7 +24236,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -24286,7 +24283,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>163</v>
       </c>
@@ -24330,7 +24327,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -24374,7 +24371,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -24418,7 +24415,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>181</v>
       </c>
@@ -24468,7 +24465,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>192</v>
       </c>
@@ -24515,7 +24512,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -24565,7 +24562,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>256</v>
       </c>
@@ -24612,7 +24609,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>202</v>
       </c>
@@ -24662,7 +24659,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -24712,7 +24709,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>95</v>
       </c>
@@ -24762,7 +24759,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -24800,7 +24797,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>211</v>
       </c>
@@ -24844,7 +24841,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>220</v>
       </c>
@@ -24894,7 +24891,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>136</v>
       </c>
@@ -24935,7 +24932,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>522</v>
       </c>
@@ -24982,7 +24979,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>105</v>
       </c>
@@ -25032,7 +25029,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>239</v>
       </c>
@@ -25073,7 +25070,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>116</v>
       </c>
@@ -25123,7 +25120,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>230</v>
       </c>
@@ -25164,7 +25161,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>126</v>
       </c>
@@ -25211,7 +25208,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>247</v>
       </c>
@@ -25278,21 +25275,21 @@
       <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.59765625" customWidth="1"/>
+    <col min="7" max="7" width="9.59765625" customWidth="1"/>
+    <col min="8" max="8" width="12.265625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1"/>
-    <col min="12" max="12" width="26.140625" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="26.265625" customWidth="1"/>
+    <col min="12" max="12" width="26.1328125" customWidth="1"/>
+    <col min="13" max="13" width="13.1328125" customWidth="1"/>
+    <col min="14" max="14" width="11.265625" customWidth="1"/>
+    <col min="15" max="15" width="16.86328125" customWidth="1"/>
+    <col min="17" max="17" width="12.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -25357,7 +25354,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>544</v>
       </c>
@@ -25407,7 +25404,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>554</v>
       </c>
@@ -25460,7 +25457,7 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>563</v>
       </c>
@@ -25501,7 +25498,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>577</v>
       </c>
@@ -25545,7 +25542,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>586</v>
       </c>
@@ -25586,7 +25583,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>602</v>
       </c>
@@ -25630,7 +25627,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>599</v>
       </c>
@@ -25671,7 +25668,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>593</v>
       </c>
@@ -25715,7 +25712,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>631</v>
       </c>
@@ -25759,7 +25756,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>624</v>
       </c>
@@ -25803,7 +25800,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>608</v>
       </c>
@@ -25853,7 +25850,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>619</v>
       </c>
@@ -25903,7 +25900,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>644</v>
       </c>
@@ -25953,7 +25950,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>639</v>
       </c>
@@ -26000,7 +25997,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>756</v>
       </c>
@@ -26047,7 +26044,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>650</v>
       </c>
@@ -26094,7 +26091,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>761</v>
       </c>
@@ -26144,7 +26141,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>728</v>
       </c>
@@ -26191,7 +26188,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>455</v>
       </c>
@@ -26241,7 +26238,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>686</v>
       </c>
@@ -26282,7 +26279,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>694</v>
       </c>
@@ -26332,7 +26329,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>703</v>
       </c>
@@ -26379,7 +26376,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>744</v>
       </c>
@@ -26423,7 +26420,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>736</v>
       </c>
@@ -26467,7 +26464,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>567</v>
       </c>
@@ -26529,7 +26526,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>679</v>
       </c>
@@ -26591,7 +26588,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>669</v>
       </c>
@@ -26644,7 +26641,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>720</v>
       </c>
@@ -26706,7 +26703,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>711</v>
       </c>
@@ -26750,7 +26747,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>658</v>
       </c>
@@ -26819,13 +26816,18 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <TaxCatchAll xmlns="be4b1b58-ad14-4d3d-90cc-b22341928211" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf1c6625-b432-47ce-9809-85c92c0fea50">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003352AD18CF0C984DA7E63E209549DCF8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7b481184ddbdf2fd96a61c5a396510c2">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf1c6625-b432-47ce-9809-85c92c0fea50" xmlns:ns3="be4b1b58-ad14-4d3d-90cc-b22341928211" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3e79b4e9e612b32c36440ec3dc8ed364" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003352AD18CF0C984DA7E63E209549DCF8" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bad55c78794288897ec35d15e0f692f4">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf1c6625-b432-47ce-9809-85c92c0fea50" xmlns:ns3="be4b1b58-ad14-4d3d-90cc-b22341928211" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c7f91d2b5b3361af338d6867d074c3f2" ns2:_="" ns3:_="">
     <xsd:import namespace="cf1c6625-b432-47ce-9809-85c92c0fea50"/>
     <xsd:import namespace="be4b1b58-ad14-4d3d-90cc-b22341928211"/>
     <xsd:element name="properties">
@@ -26846,6 +26848,8 @@
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -26910,6 +26914,13 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="d54eff52-6b6d-4e5f-a3b0-187f185b1db6" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="be4b1b58-ad14-4d3d-90cc-b22341928211" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -26939,6 +26950,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{5c6fa4d0-edc3-453b-814e-e2e662973a25}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="be4b1b58-ad14-4d3d-90cc-b22341928211">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -27050,13 +27072,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDA34A29-C3F7-4106-A9D6-21CC3D34470D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDA34A29-C3F7-4106-A9D6-21CC3D34470D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DD61DDA-75B3-4B5B-9EEE-06F2D77DE966}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15D8490A-B466-49DF-86CE-647DB4AED96D}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{753AB71A-7B2F-4035-8861-972896538258}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{753AB71A-7B2F-4035-8861-972896538258}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
tweak SSR vs SHR plots (add dashed lines for .7s)
</commit_message>
<xml_diff>
--- a/lit-search/2021-06-07-final-screening.xlsx
+++ b/lit-search/2021-06-07-final-screening.xlsx
@@ -26826,8 +26826,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003352AD18CF0C984DA7E63E209549DCF8" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bad55c78794288897ec35d15e0f692f4">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf1c6625-b432-47ce-9809-85c92c0fea50" xmlns:ns3="be4b1b58-ad14-4d3d-90cc-b22341928211" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c7f91d2b5b3361af338d6867d074c3f2" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003352AD18CF0C984DA7E63E209549DCF8" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f8c0849092bbcdbe73a73c4439cd6312">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf1c6625-b432-47ce-9809-85c92c0fea50" xmlns:ns3="be4b1b58-ad14-4d3d-90cc-b22341928211" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b842c8cf439c1c8c1011d88b1dc43cb" ns2:_="" ns3:_="">
     <xsd:import namespace="cf1c6625-b432-47ce-9809-85c92c0fea50"/>
     <xsd:import namespace="be4b1b58-ad14-4d3d-90cc-b22341928211"/>
     <xsd:element name="properties">
@@ -26850,6 +26850,8 @@
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -26920,6 +26922,16 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="23" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="24" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="be4b1b58-ad14-4d3d-90cc-b22341928211" elementFormDefault="qualified">
@@ -27081,7 +27093,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15D8490A-B466-49DF-86CE-647DB4AED96D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4810163D-4D43-428E-AED6-EC2E706A6A19}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>